<commit_message>
Analysis Results for Wikibase version of Enslaved
</commit_message>
<xml_diff>
--- a/util-scripts/NEN.csv_cq_GPT4o_results.xlsx
+++ b/util-scripts/NEN.csv_cq_GPT4o_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eziol\Documents\Indp-stdy\graph-rag-iswc-2025\util-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCD32A1-5779-4972-A4A3-AAA3A0EBC7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45779909-6B91-48D8-9C57-CF37F539D130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2988,12 +2988,6 @@
 }</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Agent record does not directly point to a hasNameRecord. I think that would have to be accessed by going from Agent to an AgentRecord. 
 To me it seems like it is treating Agent like AgentRecord. Also, seems to not be using the hasName shortcut.
 I scored this result as a 0 because the links are mostly intact between entities and relationships are mostly intact. the only issue i saw being the using the Agent entity to access name record directly instead of doing something like 
@@ -3082,6 +3076,12 @@
   </si>
   <si>
     <t>The way the model gets the ?ownershipActivity seems to not make sense to me because it looks like you'd only get the event back and not any actual details. That’s why I am rating this a -1</t>
+  </si>
+  <si>
+    <t>Score E1</t>
+  </si>
+  <si>
+    <t>Notes E1</t>
   </si>
 </sst>
 </file>
@@ -3476,8 +3476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3502,10 +3502,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -3525,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -3545,7 +3545,7 @@
         <v>-1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
@@ -3565,7 +3565,7 @@
         <v>-1</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -3585,7 +3585,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>19</v>
@@ -3605,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>27</v>
@@ -3645,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>31</v>
@@ -3665,7 +3665,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>35</v>
@@ -3685,7 +3685,7 @@
         <v>-1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>39</v>
@@ -3705,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>43</v>
@@ -3725,7 +3725,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>47</v>
@@ -3745,7 +3745,7 @@
         <v>-1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>51</v>
@@ -3765,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>55</v>
@@ -3785,7 +3785,7 @@
         <v>-1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>59</v>
@@ -3805,7 +3805,7 @@
         <v>-1</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>63</v>
@@ -3825,7 +3825,7 @@
         <v>-1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>67</v>
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>71</v>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>75</v>
@@ -3885,7 +3885,7 @@
         <v>-1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>79</v>
@@ -3905,7 +3905,7 @@
         <v>-1</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>83</v>
@@ -3925,7 +3925,7 @@
         <v>-1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>87</v>
@@ -3945,7 +3945,7 @@
         <v>-1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>91</v>
@@ -3965,7 +3965,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>95</v>
@@ -3985,7 +3985,7 @@
         <v>-1</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>99</v>

</xml_diff>